<commit_message>
Translations updates from Ida
</commit_message>
<xml_diff>
--- a/Resources_20181211.xlsx
+++ b/Resources_20181211.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EpiServer\Sites\tilsyn-automat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E315A3D0-6C57-4FEE-9668-865A66F5700F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C96820-ACB5-4EB2-8A08-AD321DA5938F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1365,8 +1365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E195"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A136" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B191" sqref="B191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>